<commit_message>
Add handling for empty data sheets
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/data_tests4.xlsx
+++ b/tests/testthat/testdata/data_tests4.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARfetchR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4856E483-B9BD-49A0-AF99-A7D9FBD49BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980FFD1C-4C55-48BC-9303-9B70823C9B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{9CD4B678-E2B4-498C-A347-770469869CC4}"/>
+    <workbookView xWindow="25080" yWindow="-1245" windowWidth="19440" windowHeight="15150" activeTab="3" xr2:uid="{9CD4B678-E2B4-498C-A347-770469869CC4}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
     <sheet name="M" sheetId="2" r:id="rId2"/>
+    <sheet name="Q" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>period</t>
   </si>
@@ -61,6 +63,12 @@
   </si>
   <si>
     <t>UMAR--MZ007--LKJ--131--A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moj </t>
+  </si>
+  <si>
+    <t>shit</t>
   </si>
 </sst>
 </file>
@@ -415,7 +423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29541F80-BAB7-4D6D-907A-8D34489C2934}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -447,7 +455,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,4 +507,41 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70A634F5-43A4-4633-8BAC-8BA8397B1A45}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4346DAFB-A5C8-488D-9728-7540D1107C0B}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>